<commit_message>
USQ Cup Part 1
</commit_message>
<xml_diff>
--- a/10v10/11/USQ-Cup/ROCHESTER_UTSA.xlsx
+++ b/10v10/11/USQ-Cup/ROCHESTER_UTSA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\live-stats\11\USQ-Cup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\10v10\11\USQ-Cup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914B3486-CED8-4EC1-A303-C90B99BEBE62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974BE5CE-BACB-4D06-9579-D0DB86B76AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="90">
   <si>
     <t>A</t>
   </si>
@@ -151,12 +153,6 @@
     <t>YB34</t>
   </si>
   <si>
-    <t>1038</t>
-  </si>
-  <si>
-    <t>?,55</t>
-  </si>
-  <si>
     <t>R1,YA37</t>
   </si>
   <si>
@@ -188,6 +184,123 @@
   </si>
   <si>
     <t>JUSTIN KING</t>
+  </si>
+  <si>
+    <t>0017</t>
+  </si>
+  <si>
+    <t>0049</t>
+  </si>
+  <si>
+    <t>0155</t>
+  </si>
+  <si>
+    <t>0224</t>
+  </si>
+  <si>
+    <t>0314</t>
+  </si>
+  <si>
+    <t>0321</t>
+  </si>
+  <si>
+    <t>0401</t>
+  </si>
+  <si>
+    <t>0501</t>
+  </si>
+  <si>
+    <t>0530</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>0619</t>
+  </si>
+  <si>
+    <t>0714</t>
+  </si>
+  <si>
+    <t>0719</t>
+  </si>
+  <si>
+    <t>0800</t>
+  </si>
+  <si>
+    <t>0817</t>
+  </si>
+  <si>
+    <t>0907</t>
+  </si>
+  <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>1026</t>
+  </si>
+  <si>
+    <t>1052</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1145</t>
+  </si>
+  <si>
+    <t>1217</t>
+  </si>
+  <si>
+    <t>1242</t>
+  </si>
+  <si>
+    <t>1258</t>
+  </si>
+  <si>
+    <t>25,55</t>
+  </si>
+  <si>
+    <t>1335</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>1528</t>
+  </si>
+  <si>
+    <t>1609</t>
+  </si>
+  <si>
+    <t>1613</t>
+  </si>
+  <si>
+    <t>1659</t>
+  </si>
+  <si>
+    <t>1718</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>1846</t>
+  </si>
+  <si>
+    <t>2029</t>
+  </si>
+  <si>
+    <t>1911</t>
+  </si>
+  <si>
+    <t>2113</t>
+  </si>
+  <si>
+    <t>2121</t>
+  </si>
+  <si>
+    <t>2126</t>
   </si>
 </sst>
 </file>
@@ -472,7 +585,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -480,20 +601,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,7 +829,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -745,21 +858,21 @@
     <row r="1" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
       <c r="R1" s="2"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -772,142 +885,142 @@
     </row>
     <row r="2" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="24">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="20">
         <f>COUNTIFS(A:A,"G*") + COUNTIFS(G:G,"G*")+COUNTIFS(M:M,"G*")+COUNTIFS(S:S,"G*")</f>
         <v>10</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="25" t="str">
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="26" t="str">
         <f>IF(COUNTIF($A$7:$X$59,"RCA"),"*","")&amp;IF(COUNTIF($A$7:$X$59,"OCA"),"^","")&amp;IF(COUNTIF($R$7:$X$59,"2CA"),"!","")</f>
         <v>*</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="16" t="str">
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="27" t="str">
         <f>CONCATENATE(LEN(O2)*30+L2*10,O2)</f>
         <v>130*</v>
       </c>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="18"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="22"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="21"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="25"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="24">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="20">
         <f>COUNTIFS(D:D,"G*")+COUNTIFS(J:J,"G*")+COUNTIFS(P:P,"G*")+COUNTIFS(V:V,"G*")</f>
         <v>8</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="25" t="str">
+      <c r="M4" s="21"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="26" t="str">
         <f>IF(COUNTIF($A$7:$R$59,"RCB"),"*","")&amp;IF(COUNTIF($A$7:$R$59,"OCB"),"^","")&amp;IF(COUNTIF($A$7:$R$59,"2CB"),"!","")</f>
         <v/>
       </c>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="16" t="str">
+      <c r="P4" s="21"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="27" t="str">
         <f>CONCATENATE(LEN(O4)*30+L4*10,O4)</f>
         <v>80</v>
       </c>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="18"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="22"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="21"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -952,22 +1065,30 @@
       <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="P7" s="6" t="s">
         <v>37</v>
       </c>
@@ -981,12 +1102,16 @@
       <c r="T7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U7" s="5"/>
+      <c r="U7" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="V7" s="6"/>
       <c r="W7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X7" s="8"/>
+      <c r="X7" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
@@ -1013,8 +1138,8 @@
       <c r="J8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>9</v>
+      <c r="K8" s="10">
+        <v>32</v>
       </c>
       <c r="L8" s="11">
         <v>1</v>
@@ -1039,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="T8" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U8" s="11">
         <v>37</v>
@@ -1089,44 +1214,60 @@
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="5"/>
+      <c r="O10" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="P10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="Q10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R10" s="8"/>
+      <c r="R10" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U10" s="5"/>
+      <c r="U10" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="V10" s="6"/>
       <c r="W10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X10" s="8"/>
+      <c r="X10" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
@@ -1176,8 +1317,8 @@
       <c r="Q11" s="10">
         <v>24</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>9</v>
+      <c r="R11" s="11">
+        <v>34</v>
       </c>
       <c r="S11" s="9" t="s">
         <v>4</v>
@@ -1185,9 +1326,7 @@
       <c r="T11" s="10">
         <v>24</v>
       </c>
-      <c r="U11" s="11">
-        <v>34</v>
-      </c>
+      <c r="U11" s="11"/>
       <c r="V11" s="9" t="s">
         <v>2</v>
       </c>
@@ -1235,44 +1374,58 @@
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U13" s="5"/>
+      <c r="U13" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="V13" s="6"/>
       <c r="W13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X13" s="8"/>
+      <c r="X13" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
@@ -1287,11 +1440,11 @@
       <c r="D14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>9</v>
+      <c r="E14" s="10">
+        <v>17</v>
+      </c>
+      <c r="F14" s="11">
+        <v>4</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>4</v>
@@ -1322,8 +1475,8 @@
       <c r="Q14" s="10">
         <v>55</v>
       </c>
-      <c r="R14" s="11" t="s">
-        <v>9</v>
+      <c r="R14" s="11">
+        <v>25</v>
       </c>
       <c r="S14" s="9" t="s">
         <v>5</v>
@@ -1377,46 +1530,62 @@
       <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="J16" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="M16" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O16" s="5"/>
+      <c r="O16" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R16" s="8"/>
+      <c r="R16" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="S16" s="3"/>
       <c r="T16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U16" s="5"/>
+      <c r="U16" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X16" s="8"/>
+      <c r="X16" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
@@ -1435,16 +1604,16 @@
         <v>37</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="H17" s="10">
+        <v>80</v>
+      </c>
+      <c r="I17" s="11">
         <v>37</v>
-      </c>
-      <c r="I17" s="11">
-        <v>80</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>10</v>
@@ -1456,10 +1625,10 @@
         <v>34</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="N17" s="10" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="N17" s="10">
+        <v>24</v>
       </c>
       <c r="O17" s="11">
         <v>33</v>
@@ -1522,57 +1691,71 @@
     </row>
     <row r="19" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="D19" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="G19" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="J19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="M19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R19" s="8"/>
+      <c r="R19" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="S19" s="3"/>
       <c r="T19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U19" s="5"/>
+      <c r="U19" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="V19" s="6"/>
       <c r="W19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X19" s="8"/>
+      <c r="X19" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
@@ -1605,8 +1788,8 @@
       <c r="J20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="10" t="s">
-        <v>9</v>
+      <c r="K20" s="10">
+        <v>4</v>
       </c>
       <c r="L20" s="11">
         <v>34</v>
@@ -28984,6 +29167,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R2:W3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="R4:W5"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
@@ -28993,13 +29183,6 @@
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:N3"/>
     <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="R2:W3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="I4:K5"/>
-    <mergeCell ref="L4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="R4:W5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -29014,7 +29197,7 @@
   </sheetPr>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
@@ -29244,7 +29427,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>28</v>
@@ -29588,7 +29771,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">

</xml_diff>